<commit_message>
- Completed changing of config files to XML, added XML files for the 8S   neck model   (note: not all of the scripts for the analysis programs work, such as   ID, FD etc)
</commit_message>
<xml_diff>
--- a/systems_prop/8S_neck_model/Neck model.xlsx
+++ b/systems_prop/8S_neck_model/Neck model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8025" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8025" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Trajectory - General" sheetId="8" r:id="rId1"/>
@@ -2903,16 +2903,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -2972,15 +2972,15 @@
         <v>0.1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C8" si="0">B2*(1/12)*(3*(0.015)^2 + 0.015^2)</f>
+        <f>B2*(1/12)*(3*(0.015)^2 + 0.015^2)</f>
         <v>7.4999999999999993E-6</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D8" si="1">B2*(1/12)*(3*(0.015)^2 + 0.015^2)</f>
+        <f t="shared" ref="D2:D8" si="0">B2*(1/12)*(3*(0.015)^2 + 0.015^2)</f>
         <v>7.4999999999999993E-6</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="2">B2*(1/2)*(0.015)^2</f>
+        <f t="shared" ref="E2:E8" si="1">B2*(1/2)*(0.015)^2</f>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F2">
@@ -3006,7 +3006,7 @@
         <v>6.4160000000000007E-3</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M8" si="3">J2+0</f>
+        <f t="shared" ref="M2:M8" si="2">J2+0</f>
         <v>0</v>
       </c>
       <c r="N2">
@@ -3034,15 +3034,15 @@
         <v>0.1</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C2:C8" si="3">B3*(1/12)*(3*(0.015)^2 + 0.015^2)</f>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D3">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F3">
@@ -3068,7 +3068,7 @@
         <v>4.3099999999999909E-4</v>
       </c>
       <c r="M3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N3">
@@ -3099,15 +3099,15 @@
         <v>0.1</v>
       </c>
       <c r="C4">
+        <f t="shared" si="3"/>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F4">
@@ -3133,7 +3133,7 @@
         <v>2.7600000000000003E-3</v>
       </c>
       <c r="M4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N4">
@@ -3164,15 +3164,15 @@
         <v>0.1</v>
       </c>
       <c r="C5">
+        <f t="shared" si="3"/>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F5">
@@ -3198,7 +3198,7 @@
         <v>2.3E-3</v>
       </c>
       <c r="M5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N5">
@@ -3229,15 +3229,15 @@
         <v>0.1</v>
       </c>
       <c r="C6">
+        <f t="shared" si="3"/>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F6">
@@ -3263,7 +3263,7 @@
         <v>5.4000000000000055E-4</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N6">
@@ -3294,15 +3294,15 @@
         <v>0.1</v>
       </c>
       <c r="C7">
+        <f t="shared" si="3"/>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F7">
@@ -3328,7 +3328,7 @@
         <v>1.4600000000000004E-3</v>
       </c>
       <c r="M7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N7">
@@ -3359,15 +3359,15 @@
         <v>0.1</v>
       </c>
       <c r="C8">
+        <f t="shared" si="3"/>
+        <v>7.4999999999999993E-6</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>7.4999999999999993E-6</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="1"/>
-        <v>7.4999999999999993E-6</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
         <v>1.1250000000000001E-5</v>
       </c>
       <c r="F8">
@@ -3393,7 +3393,7 @@
         <v>8.9999999999999802E-4</v>
       </c>
       <c r="M8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N8">
@@ -3488,7 +3488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D39" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>